<commit_message>
Started commits from here
</commit_message>
<xml_diff>
--- a/Rokomari_TestCase.xlsx
+++ b/Rokomari_TestCase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fariha/Desktop/DESKTOP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fariha/Desktop/GitRep/SQA_Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23316F84-2FEC-C642-AA2F-E4A7E23AC196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C116C54-54D2-0C45-AC1A-A2F24FF0454F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,12 +246,6 @@
     <t>Pre Condition</t>
   </si>
   <si>
-    <t xml:space="preserve">1.Must be Small letter without space.
-2.Between @ and dot (.) there must be a valid Email Providers
-3.There must be a valid domain after dot.
-</t>
-  </si>
-  <si>
     <t>1.Must be Small letter without space.
 2.Between @ and dot (.) there must be a valid Email Providers
 3.There must be a valid domain after dot.</t>
@@ -261,6 +255,12 @@
 2.Click on Sign Up Option
 3.Enter The Valid Email
 4.Click On The Sign In Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Must be Small letter without space.
+2.Between @ and dot (.) there must be a valid Email Providers
+3.There must be a valid domain after dot. 
+</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -892,13 +892,13 @@
         <v>52</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16" t="s">
@@ -917,7 +917,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>34</v>
@@ -944,7 +944,7 @@
         <v>35</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>36</v>
@@ -970,7 +970,7 @@
         <v>39</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>38</v>
@@ -993,7 +993,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>40</v>
@@ -1014,7 +1014,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>42</v>
@@ -1037,7 +1037,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>44</v>

</xml_diff>